<commit_message>
resolved typo in source properties generator script
</commit_message>
<xml_diff>
--- a/dbt_project_setup_automation/ip/data_dictionary_data_src_eg.xlsx
+++ b/dbt_project_setup_automation/ip/data_dictionary_data_src_eg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulfry/Dropbox/tech/code/git-repos/dbt_repos/dbt/dbt_project_setup_automation/ip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851E9625-CA99-A34B-9FE1-388D8CF8121D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E61A13-A927-C84A-A40A-549EEA69AFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{F5447BD4-51BA-CB4A-AA03-46A64813458D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{F5447BD4-51BA-CB4A-AA03-46A64813458D}"/>
   </bookViews>
   <sheets>
     <sheet name="data_src_a_table_a" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="24">
   <si>
     <t>unique_key</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>a,b,c</t>
+  </si>
+  <si>
+    <t>comments</t>
   </si>
 </sst>
 </file>
@@ -202,9 +205,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D8B9D1A0-C2F8-994C-A038-F683BB3EAAE9}" name="Table2" displayName="Table2" ref="B3:J7" totalsRowShown="0">
-  <autoFilter ref="B3:J7" xr:uid="{D8B9D1A0-C2F8-994C-A038-F683BB3EAAE9}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D8B9D1A0-C2F8-994C-A038-F683BB3EAAE9}" name="Table2" displayName="Table2" ref="B3:K7" totalsRowShown="0">
+  <autoFilter ref="B3:K7" xr:uid="{D8B9D1A0-C2F8-994C-A038-F683BB3EAAE9}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{72D067D0-8E61-8546-B65D-7F7FF631A866}" name="no"/>
     <tableColumn id="2" xr3:uid="{DB1DC045-AFC3-DF49-AC9B-4C31084BA7B9}" name="table"/>
     <tableColumn id="3" xr3:uid="{5CDBA1C4-4CF5-CD45-9FBF-36494DEC28CB}" name="field"/>
@@ -214,15 +217,16 @@
     <tableColumn id="7" xr3:uid="{26664B8F-5D74-0642-9DF6-0B6BD53CA600}" name="accepted_values"/>
     <tableColumn id="8" xr3:uid="{E8BCB4A9-267A-C341-9095-2399C9E2376C}" name="fk_contraint_table"/>
     <tableColumn id="9" xr3:uid="{27D65D4C-E4B2-DE4C-8180-F043DE421F54}" name="fk_contraint_key"/>
+    <tableColumn id="10" xr3:uid="{1CE9CB1E-0B30-D24A-B28D-276FA8E1645A}" name="comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B4B325D8-FB0F-0342-964F-517F4E3F298B}" name="Table24" displayName="Table24" ref="B3:J6" totalsRowShown="0">
-  <autoFilter ref="B3:J6" xr:uid="{D8B9D1A0-C2F8-994C-A038-F683BB3EAAE9}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B4B325D8-FB0F-0342-964F-517F4E3F298B}" name="Table24" displayName="Table24" ref="B3:K6" totalsRowShown="0">
+  <autoFilter ref="B3:K6" xr:uid="{D8B9D1A0-C2F8-994C-A038-F683BB3EAAE9}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{7CF1B6FB-CEBC-B54B-9E7A-3BE1AE2E3C17}" name="no"/>
     <tableColumn id="2" xr3:uid="{22A6305B-EF5E-4541-BAB2-7901F6582337}" name="table"/>
     <tableColumn id="3" xr3:uid="{F87EAFF0-4ABE-0F46-8960-20A0CC25DFB5}" name="field"/>
@@ -232,6 +236,7 @@
     <tableColumn id="7" xr3:uid="{13995F2A-884C-EC4C-91AE-A78AA7FC7811}" name="accepted_values"/>
     <tableColumn id="8" xr3:uid="{597F6071-F050-CE46-B51A-EB42F8533BB0}" name="fk_contraint_table"/>
     <tableColumn id="9" xr3:uid="{20F9BD36-5CC9-D54C-832F-15B82B1B6FE9}" name="fk_contraint_key"/>
+    <tableColumn id="10" xr3:uid="{449E05AD-1F24-5448-B133-C7F721CABBBC}" name="comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -534,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A3F06E-3DE3-9748-8162-6D49E20586D1}">
-  <dimension ref="B2:J7"/>
+  <dimension ref="B2:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,9 +555,10 @@
     <col min="8" max="8" width="17.1640625" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
@@ -563,7 +569,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -591,8 +597,11 @@
       <c r="J3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1</v>
       </c>
@@ -615,7 +624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>2</v>
       </c>
@@ -632,7 +641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" ht="34" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>3</v>
       </c>
@@ -649,7 +658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" ht="34" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>4</v>
       </c>
@@ -683,10 +692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E301CF-5EFF-2C41-B661-9A4150B69AC2}">
-  <dimension ref="B2:J6"/>
+  <dimension ref="B2:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,9 +708,10 @@
     <col min="8" max="8" width="17.1640625" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
@@ -711,8 +721,9 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -740,8 +751,11 @@
       <c r="J3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1</v>
       </c>
@@ -764,7 +778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>2</v>
       </c>
@@ -781,7 +795,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" ht="34" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>4</v>
       </c>
@@ -807,7 +821,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>